<commit_message>
New sheet for the core uk version
</commit_message>
<xml_diff>
--- a/summary_questions.xlsx
+++ b/summary_questions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="UK pilot" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="UK pilot - 2016" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Core Version - 2017" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="231">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -373,6 +373,33 @@
     <t xml:space="preserve">Do you provide help and expertise in software development to researchers from across your organisation?</t>
   </si>
   <si>
+    <t xml:space="preserve">currentWORKCANADA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If no, is there such a group within your organization?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if no to currentWork1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currentWorkCan1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If no, do you think such a group would have value?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if no to currentWorkCAN1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currentWorkCan2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If yes, would you be interested in participating in such a group?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if no to currentWorkCAN2</t>
+  </si>
+  <si>
     <t xml:space="preserve">currentWork2</t>
   </si>
   <si>
@@ -434,6 +461,21 @@
   </si>
   <si>
     <t xml:space="preserve">if no to paper4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conf1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have you ever presented your software work at a conference or workshop? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conf2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If yes, which conference(s)/workshop(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if yes to con1</t>
   </si>
   <si>
     <t xml:space="preserve">stability1</t>
@@ -786,7 +828,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -867,6 +909,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -877,6 +927,26 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -896,7 +966,6 @@
         <family val="2"/>
         <color rgb="FF000000"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -967,25 +1036,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K78"/>
+  <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D75" activeCellId="0" sqref="D75"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A74" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A83" activeCellId="0" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.69767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="14.906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="63.2604651162791"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.0325581395349"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.5767441860465"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="32.2837209302326"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.1953488372093"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="66.6279069767442"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.5441860465116"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="76.3813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="13.4651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.24651162790698"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="16.0697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="68.2"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.2697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.4046511627907"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="34.753488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.5767441860465"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="71.7767441860465"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="82.353488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="14.4976744186047"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1232,25 +1301,29 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0"/>
       <c r="B9" s="0"/>
       <c r="C9" s="15"/>
       <c r="D9" s="10"/>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
+      <c r="G9" s="0"/>
       <c r="H9" s="0"/>
+      <c r="I9" s="0"/>
       <c r="J9" s="0"/>
       <c r="K9" s="0"/>
     </row>
-    <row r="10" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
       <c r="B10" s="0"/>
       <c r="C10" s="15"/>
       <c r="D10" s="10"/>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
+      <c r="G10" s="0"/>
       <c r="H10" s="0"/>
+      <c r="I10" s="0"/>
       <c r="J10" s="0"/>
       <c r="K10" s="0"/>
     </row>
@@ -1920,7 +1993,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" s="20" customFormat="true" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" s="20" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="20" t="n">
         <v>4</v>
       </c>
@@ -1939,161 +2012,131 @@
       <c r="H34" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="I34" s="22"/>
-      <c r="J34" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="K34" s="20" t="s">
+    </row>
+    <row r="35" s="20" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="20" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="35" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4" t="n">
+      <c r="D35" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="H35" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" s="20" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="H36" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" s="22" customFormat="true" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="D35" s="10"/>
-    </row>
-    <row r="36" s="9" customFormat="true" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J36" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" s="9" customFormat="true" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="E37" s="6" t="s">
+      <c r="C37" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="E37" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="F37" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J37" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" s="4" customFormat="true" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G37" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="H37" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I37" s="24"/>
+      <c r="J37" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="K37" s="22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="E38" s="4" t="s">
+      <c r="D38" s="10"/>
+    </row>
+    <row r="39" s="9" customFormat="true" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J39" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" s="9" customFormat="true" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I39" s="0"/>
-      <c r="J39" s="0"/>
-      <c r="K39" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B40" s="0"/>
-      <c r="C40" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I40" s="0"/>
-      <c r="J40" s="0"/>
-      <c r="K40" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F40" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J40" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" s="4" customFormat="true" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="C41" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="D41" s="10" t="s">
         <v>134</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>135</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>37</v>
@@ -2101,150 +2144,157 @@
       <c r="F41" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G41" s="4" t="s">
-        <v>136</v>
-      </c>
       <c r="H41" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I41" s="0"/>
-      <c r="J41" s="0"/>
       <c r="K41" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="42" s="9" customFormat="true" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6" t="s">
+      <c r="B42" s="4"/>
+      <c r="C42" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D42" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="E42" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E42" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" s="9" customFormat="true" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="6" t="n">
+      <c r="H42" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" s="0"/>
+      <c r="J42" s="0"/>
+      <c r="K42" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6" t="s">
+      <c r="B43" s="0"/>
+      <c r="C43" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E43" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F43" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6" t="s">
+      <c r="F43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="H43" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I43" s="0"/>
+      <c r="J43" s="0"/>
+      <c r="K43" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B44" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="C44" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="F44" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6" t="s">
-        <v>21</v>
+      <c r="D44" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="I44" s="0"/>
       <c r="J44" s="0"/>
-      <c r="K44" s="0"/>
-    </row>
-    <row r="45" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I45" s="0"/>
-      <c r="J45" s="0"/>
-      <c r="K45" s="0"/>
-    </row>
-    <row r="46" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6" t="s">
+      <c r="K44" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" s="25" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C45" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D45" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="E46" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I46" s="0"/>
-      <c r="J46" s="0"/>
-      <c r="K46" s="0"/>
-    </row>
-    <row r="47" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E45" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="K45" s="20"/>
+    </row>
+    <row r="46" s="25" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="H46" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="K46" s="20"/>
+    </row>
+    <row r="47" s="9" customFormat="true" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B47" s="6"/>
       <c r="C47" s="6" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>143</v>
+        <v>152</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>11</v>
@@ -2253,23 +2303,20 @@
       <c r="H47" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I47" s="0"/>
-      <c r="J47" s="0"/>
-      <c r="K47" s="0"/>
-    </row>
-    <row r="48" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="48" s="9" customFormat="true" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B48" s="6"/>
       <c r="C48" s="6" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>143</v>
+        <v>154</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>11</v>
@@ -2278,9 +2325,6 @@
       <c r="H48" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I48" s="0"/>
-      <c r="J48" s="0"/>
-      <c r="K48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="n">
@@ -2288,13 +2332,13 @@
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="6" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>11</v>
@@ -2313,13 +2357,13 @@
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="6" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>11</v>
@@ -2338,13 +2382,13 @@
       </c>
       <c r="B51" s="6"/>
       <c r="C51" s="6" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D51" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="E51" s="9" t="s">
         <v>157</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>143</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>11</v>
@@ -2357,19 +2401,19 @@
       <c r="J51" s="0"/>
       <c r="K51" s="0"/>
     </row>
-    <row r="52" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="n">
         <v>5</v>
       </c>
       <c r="B52" s="6"/>
       <c r="C52" s="6" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>11</v>
@@ -2382,19 +2426,19 @@
       <c r="J52" s="0"/>
       <c r="K52" s="0"/>
     </row>
-    <row r="53" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="n">
         <v>5</v>
       </c>
       <c r="B53" s="6"/>
       <c r="C53" s="6" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>11</v>
@@ -2413,13 +2457,13 @@
       </c>
       <c r="B54" s="6"/>
       <c r="C54" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>11</v>
@@ -2432,19 +2476,19 @@
       <c r="J54" s="0"/>
       <c r="K54" s="0"/>
     </row>
-    <row r="55" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="n">
         <v>5</v>
       </c>
       <c r="B55" s="6"/>
       <c r="C55" s="6" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>11</v>
@@ -2463,13 +2507,13 @@
       </c>
       <c r="B56" s="6"/>
       <c r="C56" s="6" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>11</v>
@@ -2482,19 +2526,19 @@
       <c r="J56" s="0"/>
       <c r="K56" s="0"/>
     </row>
-    <row r="57" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="n">
         <v>5</v>
       </c>
       <c r="B57" s="6"/>
       <c r="C57" s="6" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>11</v>
@@ -2507,19 +2551,19 @@
       <c r="J57" s="0"/>
       <c r="K57" s="0"/>
     </row>
-    <row r="58" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="n">
         <v>5</v>
       </c>
       <c r="B58" s="6"/>
       <c r="C58" s="6" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>11</v>
@@ -2538,13 +2582,13 @@
       </c>
       <c r="B59" s="6"/>
       <c r="C59" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>11</v>
@@ -2557,19 +2601,19 @@
       <c r="J59" s="0"/>
       <c r="K59" s="0"/>
     </row>
-    <row r="60" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="6" t="n">
         <v>5</v>
       </c>
       <c r="B60" s="6"/>
       <c r="C60" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>11</v>
@@ -2588,13 +2632,13 @@
       </c>
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>11</v>
@@ -2613,13 +2657,13 @@
       </c>
       <c r="B62" s="6"/>
       <c r="C62" s="6" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D62" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E62" s="9" t="s">
         <v>180</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>11</v>
@@ -2632,19 +2676,19 @@
       <c r="J62" s="0"/>
       <c r="K62" s="0"/>
     </row>
-    <row r="63" customFormat="false" ht="26.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="n">
         <v>5</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>11</v>
@@ -2657,19 +2701,19 @@
       <c r="J63" s="0"/>
       <c r="K63" s="0"/>
     </row>
-    <row r="64" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="n">
         <v>5</v>
       </c>
       <c r="B64" s="6"/>
       <c r="C64" s="6" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>11</v>
@@ -2688,13 +2732,13 @@
       </c>
       <c r="B65" s="6"/>
       <c r="C65" s="6" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>11</v>
@@ -2707,19 +2751,19 @@
       <c r="J65" s="0"/>
       <c r="K65" s="0"/>
     </row>
-    <row r="66" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="n">
         <v>5</v>
       </c>
       <c r="B66" s="6"/>
       <c r="C66" s="6" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>11</v>
@@ -2732,19 +2776,19 @@
       <c r="J66" s="0"/>
       <c r="K66" s="0"/>
     </row>
-    <row r="67" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="n">
         <v>5</v>
       </c>
       <c r="B67" s="6"/>
       <c r="C67" s="6" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>11</v>
@@ -2757,19 +2801,19 @@
       <c r="J67" s="0"/>
       <c r="K67" s="0"/>
     </row>
-    <row r="68" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="26.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="n">
         <v>5</v>
       </c>
       <c r="B68" s="6"/>
       <c r="C68" s="6" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>11</v>
@@ -2788,13 +2832,13 @@
       </c>
       <c r="B69" s="6"/>
       <c r="C69" s="6" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>11</v>
@@ -2809,17 +2853,17 @@
     </row>
     <row r="70" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B70" s="6"/>
       <c r="C70" s="6" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>197</v>
+        <v>200</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>180</v>
       </c>
       <c r="F70" s="6" t="s">
         <v>11</v>
@@ -2832,19 +2876,19 @@
       <c r="J70" s="0"/>
       <c r="K70" s="0"/>
     </row>
-    <row r="71" customFormat="false" ht="39.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B71" s="6"/>
       <c r="C71" s="6" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>197</v>
+        <v>202</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>180</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>11</v>
@@ -2857,19 +2901,19 @@
       <c r="J71" s="0"/>
       <c r="K71" s="0"/>
     </row>
-    <row r="72" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B72" s="6"/>
       <c r="C72" s="6" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>197</v>
+        <v>204</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>180</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>11</v>
@@ -2884,17 +2928,17 @@
     </row>
     <row r="73" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="6" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>14</v>
+        <v>206</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>180</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>11</v>
@@ -2909,17 +2953,17 @@
     </row>
     <row r="74" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B74" s="6"/>
       <c r="C74" s="6" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>14</v>
+        <v>208</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>180</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>11</v>
@@ -2928,45 +2972,36 @@
       <c r="H74" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I74" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="J74" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="I74" s="0"/>
+      <c r="J74" s="0"/>
       <c r="K74" s="0"/>
     </row>
-    <row r="75" s="11" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="14" t="n">
+    <row r="75" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="B75" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="C75" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="D75" s="13" t="s">
+      <c r="B75" s="6"/>
+      <c r="C75" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="E75" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G75" s="14"/>
-      <c r="H75" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="I75" s="14" t="s">
+      <c r="D75" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="J75" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="K75" s="14" t="s">
+      <c r="E75" s="6" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="76" s="9" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F75" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I75" s="0"/>
+      <c r="J75" s="0"/>
+      <c r="K75" s="0"/>
+    </row>
+    <row r="76" customFormat="false" ht="39.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="n">
         <v>6</v>
       </c>
@@ -2978,7 +3013,7 @@
         <v>213</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>14</v>
+        <v>211</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>11</v>
@@ -2987,25 +3022,23 @@
       <c r="H76" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I76" s="6"/>
-      <c r="J76" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K76" s="6"/>
-    </row>
-    <row r="77" s="9" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I76" s="0"/>
+      <c r="J76" s="0"/>
+      <c r="K76" s="0"/>
+    </row>
+    <row r="77" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="n">
         <v>6</v>
       </c>
       <c r="B77" s="6"/>
       <c r="C77" s="6" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>14</v>
+        <v>211</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>11</v>
@@ -3014,25 +3047,23 @@
       <c r="H77" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I77" s="6"/>
-      <c r="J77" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K77" s="6"/>
-    </row>
-    <row r="78" s="9" customFormat="true" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I77" s="0"/>
+      <c r="J77" s="0"/>
+      <c r="K77" s="0"/>
+    </row>
+    <row r="78" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="n">
         <v>6</v>
       </c>
       <c r="B78" s="6"/>
       <c r="C78" s="6" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>11</v>
@@ -3041,18 +3072,156 @@
       <c r="H78" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I78" s="6"/>
-      <c r="J78" s="6"/>
-      <c r="K78" s="6"/>
+      <c r="I78" s="0"/>
+      <c r="J78" s="0"/>
+      <c r="K78" s="0"/>
+    </row>
+    <row r="79" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I79" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="J79" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K79" s="0"/>
+    </row>
+    <row r="80" s="11" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="B80" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="C80" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="D80" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="E80" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G80" s="14"/>
+      <c r="H80" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I80" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="J80" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K80" s="14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="81" s="9" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K81" s="6"/>
+    </row>
+    <row r="82" s="9" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K82" s="6"/>
+    </row>
+    <row r="83" s="9" customFormat="true" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C34">
+  <conditionalFormatting sqref="C37">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>$H34=same</formula>
+      <formula>$H37=same</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="I75" r:id="rId1" display="https://www.academia.edu/1112558/Comparative_study_on_the_collection_of_data_to_measure_the_extent_and_impact_of_discrimination_within_the_United_States_Canada_Australia_the_United_Kingdom_and_the_Netherlands"/>
+    <hyperlink ref="I80" r:id="rId1" display="https://www.academia.edu/1112558/Comparative_study_on_the_collection_of_data_to_measure_the_extent_and_impact_of_discrimination_within_the_United_States_Canada_Australia_the_United_Kingdom_and_the_Netherlands"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0.39375" bottom="0.39375" header="0" footer="0"/>
@@ -3069,14 +3238,1646 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="1:73"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <sheetData/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="6.70232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="14.1674418604651"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="14.9953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="25" width="54.0558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="25" width="15.6883720930233"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="25" width="8.93488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="25" width="28.9627906976744"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="25" width="20.8697674418605"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="25" width="23.9813953488372"/>
+    <col collapsed="false" hidden="false" max="1023" min="10" style="25" width="8.93488372093023"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="26"/>
+      <c r="H2" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AMJ2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="AMJ4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="AMJ8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="20" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="20" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="20" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="20" t="n">
+        <v>2</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="AMJ13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="20" t="n">
+        <v>2</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="20" t="n">
+        <v>2</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AMJ15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="20" t="n">
+        <v>2</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="20" t="n">
+        <v>2</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="AMJ17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="20" t="n">
+        <v>2</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="20"/>
+      <c r="I18" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="20" t="n">
+        <v>2</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="20" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="I22" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="AMJ23" s="0"/>
+    </row>
+    <row r="24" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="AMJ24" s="0"/>
+    </row>
+    <row r="25" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="AMJ25" s="0"/>
+    </row>
+    <row r="26" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="AMJ26" s="0"/>
+    </row>
+    <row r="27" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="H27" s="25"/>
+      <c r="I27" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="AMJ27" s="0"/>
+    </row>
+    <row r="28" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="D28" s="28"/>
+      <c r="AMJ28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I29" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="AMJ31" s="0"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="J32" s="20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="J33" s="20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="D34" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="J34" s="20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="J35" s="20"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="J36" s="20"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="20"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="20"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="D39" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="E39" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="20"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="20"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="D41" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="E41" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="20"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="D42" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="F42" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="20"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="D43" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="E43" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="20"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="D44" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="E44" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="F44" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="20"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="D45" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="E45" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="F45" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="20"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="D46" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="E46" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="20"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="D47" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E47" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="F47" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="20"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="D48" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="E48" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="F48" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="20"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="D49" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="F49" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G49" s="20"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="D50" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="E50" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F50" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" s="20"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="D51" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="E51" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F51" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" s="20"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B52" s="20"/>
+      <c r="C52" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="D52" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="E52" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F52" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" s="20"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="D53" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="E53" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F53" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G53" s="20"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="D54" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="E54" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F54" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G54" s="20"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B55" s="20"/>
+      <c r="C55" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="D55" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="E55" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F55" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55" s="20"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="D56" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="E56" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F56" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G56" s="20"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B57" s="20"/>
+      <c r="C57" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="D57" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="E57" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F57" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G57" s="20"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B58" s="20"/>
+      <c r="C58" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="D58" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="E58" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F58" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G58" s="20"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B59" s="20"/>
+      <c r="C59" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D59" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="E59" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" s="20"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B60" s="20"/>
+      <c r="C60" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="D60" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="E60" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G60" s="20"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B61" s="20"/>
+      <c r="C61" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="D61" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="E61" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F61" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G61" s="20"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B62" s="20"/>
+      <c r="C62" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="D62" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="E62" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F62" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G62" s="20"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B63" s="20"/>
+      <c r="C63" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="D63" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="E63" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F63" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G63" s="20"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B64" s="20"/>
+      <c r="C64" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="D64" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="E64" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F64" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G64" s="20"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="20" t="n">
+        <v>6</v>
+      </c>
+      <c r="B65" s="20"/>
+      <c r="C65" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D65" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="E65" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F65" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G65" s="20"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="20" t="n">
+        <v>6</v>
+      </c>
+      <c r="B66" s="20"/>
+      <c r="C66" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="D66" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="E66" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F66" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G66" s="20"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="20" t="n">
+        <v>6</v>
+      </c>
+      <c r="B67" s="20"/>
+      <c r="C67" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="D67" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="E67" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F67" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G67" s="20"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="20" t="n">
+        <v>6</v>
+      </c>
+      <c r="B68" s="20"/>
+      <c r="C68" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="D68" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="E68" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F68" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G68" s="20"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="20" t="n">
+        <v>6</v>
+      </c>
+      <c r="B69" s="20"/>
+      <c r="C69" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="D69" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="E69" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F69" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G69" s="20"/>
+      <c r="H69" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="I69" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="20" t="n">
+        <v>6</v>
+      </c>
+      <c r="B70" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="C70" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="D70" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="E70" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G70" s="20"/>
+      <c r="H70" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="I70" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="J70" s="20" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="20" t="n">
+        <v>6</v>
+      </c>
+      <c r="B71" s="20"/>
+      <c r="C71" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="D71" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="E71" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F71" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G71" s="20"/>
+      <c r="H71" s="20"/>
+      <c r="I71" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="J71" s="20"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="20" t="n">
+        <v>6</v>
+      </c>
+      <c r="B72" s="20"/>
+      <c r="C72" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="D72" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="E72" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F72" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G72" s="20"/>
+      <c r="H72" s="20"/>
+      <c r="I72" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="J72" s="20"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="20" t="n">
+        <v>6</v>
+      </c>
+      <c r="B73" s="20"/>
+      <c r="C73" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="D73" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="E73" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F73" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G73" s="20"/>
+      <c r="H73" s="20"/>
+      <c r="I73" s="20"/>
+      <c r="J73" s="20"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>#REF!=same</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="H70" r:id="rId1" display="https://www.academia.edu/1112558/Comparative_study_on_the_collection_of_data_to_measure_the_extent_and_impact_of_discrimination_within_the_United_States_Canada_Australia_the_United_Kingdom_and_the_Netherlands"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added draft from canada
</commit_message>
<xml_diff>
--- a/summary_questions.xlsx
+++ b/summary_questions.xlsx
@@ -9,7 +9,8 @@
   </bookViews>
   <sheets>
     <sheet name="UK pilot - 2016" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Core Version - 2017" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Canada -- First draft" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Core Version - 2017" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,8 +21,60 @@
 </workbook>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C45" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Scott Henwood:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Hard to draw any conclusions in an anonymous survey</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D74" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Scott Henwood: 
+This is an SSI question. Kathryn had some concerns about its clarity, but I asked some of the technical people in the office and they were all comfortable with it.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="323">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -716,6 +769,282 @@
   </si>
   <si>
     <t xml:space="preserve">Are you a member of the UK RSE Association? (Members are people who have signed up to the UK RSE mailing list)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSI Ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMF Ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Answers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Why am I asking this</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What percentage of your time is spent on research?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What percentage of the time you spend writing software is spent on new development/enhancement?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What percentage of the time you spend writing software is devoted to maintenance and support activities?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How many years of software development experience do you have?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you consider yourself a professional software developer?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y/N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How many software projects are you currently involved in?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How many software developers typically work on your projects?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just me, 2, 3-5, 6-9, 10+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What percentage of these developers are dedicated to the project full time?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How are your projects typically tested (check all that apply)? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No formal testing, the developers do their own testing, dedicated test engineers, user testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do your research software projects typically include a project manager?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What development methodology does your current project use?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waterfall, Scrum, Kanban, other, no formal methodology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;list&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What percentage of the software projects you've worked on are released under an open source license?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List any open repositories (eg. GitHub) to which your software projects have been published.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RDC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What percentage of the software projects you've worked on have an associated Digital Object Identifier (DOI)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What programming languages do you use in developing research software? Please list in order, beginning with most frequently used.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What platform(s) are your research software projects deployed on (check all that apply)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compute Canada HPC, University compute centre, Other HPC, Cloud, Stand-alone server(s), Laptop/desktop, Mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI-51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do any of your current projects make use of a data management or data archiving component?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If yes, is it part of your software or an external system (please specify)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check boxes with text field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do any of your current projects accommodate the open/public sharing of data?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If yes, is the creation of a Digital Object Identifier (DOI) and metadata for individual assets supported?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Would you be interested in joining such an organization if one was formed in Canada?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What would you hope to get out of such an organization (check all that apply)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Networking, software collaborations, research collaborations, training, research software standards and interoperability definition, job opportunities, other(specify)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How is your current research software work funded?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employer, CANARIE, CFI, CIHR, Genome Canada, NSERC, SSHRC, Don't know, Other (specify)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Who else should be aware of this survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have you developed software that is accessed from multiple institutions?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do any of your current or previous projects make use of the Canadian Access Federation (CAF) Federated Identity Management (FIM) service?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List any public identity providers (Google, Facebook, Live, LinkedIn, Twitter etc.) used in your current or previous projects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drives PI-44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have you ever visited the research software registry at science.canarie.ca?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blatent marketing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI-43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How many software components from science.canarie.ca have you integrated into your projects?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">socio 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you work in Canada?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identify target audience</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rse 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you write software for research as part of your job?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edu 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the highest level of education you have attained?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High School, Some College, College Diploma, Some University, Bachelors Degree, Masters Degree, Doctorate, Other, None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understand the background of research software developers to understand training needs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edu 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In which discipline is your highest academic qualification?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSERC Codes + Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edu 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List any professional qualifications you hold (eg. P. Eng, PMP, …)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rse 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What percentage of your time is spent developing software?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understand research software development practices to see what efficiencies from commercial software development we can encourage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What type of organization do you work for?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University, college, non-profit, charity, government department, private sector, other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understand if we need to expand community beyond universities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is your current job title?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;text&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Determine how we might be able to identify members of this community so we can communicate with them</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In which application area do you primarily work?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSERC Codes + Multi-discipline + Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combine with experience questions to identify disciplines that could benefit from professional software developers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the nature of your current employment?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full-time, part-time, co-op/intern, grad student, post doc, contract, consultant, self-employed, other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speaks to the efficiency of software development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you work within a group that provides software development help or expertise to researchers from across your organization?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follow up on feedback from outreach suggesting that such a group is a good idea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have you contributed software to research that has been published in a journal or presented at a conference?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understand how software is seen by the research community in Canada. This is useful for comparison to other countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In your opinion, what are the three most important skills that a Research Software Developer must possess? These skills can be technical and non-technical.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identify areas for presentation at future workshops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What three skills would you like to acquire or improve to help your work as a Research Software Developer? These skills can be technical and non-technical.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are the three tools or services you use most often in your software work?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understanding the skillset and where the CANARIE team might be able to add value. Also understand what servcices might have greatest impact.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is your Operating System of choice for deployment?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNU/Linux, Mac OS, Windows, iOS, Android, Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are you a member of an association of Research Software Developers (UK RSE, for example)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Determine if there is there a benefit to us supporting the creation of such an organization</t>
   </si>
 </sst>
 </file>
@@ -725,7 +1054,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -752,6 +1081,50 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF4472C4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFED7D31"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -784,7 +1157,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF9900"/>
-        <bgColor rgb="FFFFCC00"/>
+        <bgColor rgb="FFED7D31"/>
       </patternFill>
     </fill>
     <fill>
@@ -828,7 +1201,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -933,6 +1306,54 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1010,12 +1431,12 @@
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF4472C4"/>
       <rgbColor rgb="FF33FF99"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFED7D31"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -1039,7 +1460,7 @@
   <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A74" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A83" activeCellId="0" sqref="A83"/>
+      <selection pane="topLeft" activeCell="A83" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3238,10 +3659,877 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:K77"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.646511627907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="26" width="17.646511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="26" width="13.8093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="119.493023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="21" width="85.5767441860465"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="14.2186046511628"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="14.2186046511628"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="29" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0"/>
+      <c r="B1" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
+      <c r="D2" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="F2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="F3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0"/>
+      <c r="C4" s="0"/>
+      <c r="D4" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="F4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0"/>
+      <c r="C5" s="0"/>
+      <c r="F5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="F6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0"/>
+      <c r="C7" s="0"/>
+      <c r="D7" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="F7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
+      <c r="F8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0"/>
+      <c r="C9" s="0"/>
+      <c r="D9" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="F9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0"/>
+      <c r="C10" s="0"/>
+      <c r="D10" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="F10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0"/>
+      <c r="C11" s="0"/>
+      <c r="D11" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="F11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0"/>
+      <c r="C12" s="0"/>
+      <c r="F12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="F13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
+      <c r="D14" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="F14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="30.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+      <c r="D15" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="F15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0"/>
+      <c r="C16" s="0"/>
+      <c r="D16" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="F16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
+      <c r="D17" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="F17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="F18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
+      <c r="D20" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="F20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0"/>
+      <c r="C21" s="0"/>
+      <c r="D21" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="F21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0"/>
+      <c r="C22" s="0"/>
+      <c r="D22" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="F22" s="0"/>
+    </row>
+    <row r="23" s="32" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="E23" s="31" t="s">
+        <v>252</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="24" s="34" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="F24" s="31" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+      <c r="D25" s="0"/>
+      <c r="E25" s="0"/>
+      <c r="F25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0"/>
+      <c r="C26" s="0"/>
+      <c r="D26" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="F26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0"/>
+      <c r="C27" s="0"/>
+      <c r="D27" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="F27" s="0"/>
+    </row>
+    <row r="28" s="34" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="31" t="s">
+        <v>260</v>
+      </c>
+      <c r="D28" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="E28" s="31" t="s">
+        <v>242</v>
+      </c>
+      <c r="F28" s="31" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="29" s="34" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="F29" s="31" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="30" s="34" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="31" t="s">
+        <v>260</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>242</v>
+      </c>
+      <c r="F30" s="31" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" s="34" customFormat="true" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>242</v>
+      </c>
+      <c r="F31" s="31" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0"/>
+      <c r="C32" s="0"/>
+      <c r="D32" s="0"/>
+      <c r="E32" s="0"/>
+      <c r="F32" s="0"/>
+    </row>
+    <row r="34" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D34" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="F34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D35" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="F35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D36" s="0"/>
+      <c r="E36" s="0"/>
+      <c r="F36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D37" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="F37" s="26" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
+      <c r="F38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D39" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="E39" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="F39" s="36" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D40" s="35" t="s">
+        <v>274</v>
+      </c>
+      <c r="E40" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="F40" s="36" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D41" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="E41" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="F41" s="36" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D42" s="35"/>
+      <c r="F42" s="36" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0"/>
+      <c r="C44" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="F44" s="26" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0"/>
+      <c r="C45" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="F45" s="0"/>
+    </row>
+    <row r="52" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="37"/>
+      <c r="B52" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="C52" s="37"/>
+      <c r="D52" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="G52" s="37"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="37"/>
+      <c r="J52" s="37"/>
+      <c r="K52" s="37"/>
+    </row>
+    <row r="53" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="37"/>
+      <c r="B53" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="C53" s="37"/>
+      <c r="D53" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="F53" s="37"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="37"/>
+      <c r="J53" s="37"/>
+      <c r="K53" s="37"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="37"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="37"/>
+      <c r="J54" s="37"/>
+      <c r="K54" s="37"/>
+    </row>
+    <row r="55" customFormat="false" ht="89.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="37"/>
+      <c r="B55" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="C55" s="37"/>
+      <c r="D55" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="E55" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="F55" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="G55" s="37"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="37"/>
+      <c r="J55" s="37"/>
+      <c r="K55" s="37"/>
+    </row>
+    <row r="56" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="37"/>
+      <c r="B56" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="C56" s="37"/>
+      <c r="D56" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="E56" s="21" t="s">
+        <v>292</v>
+      </c>
+      <c r="F56" s="37"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="37"/>
+      <c r="J56" s="37"/>
+      <c r="K56" s="37"/>
+    </row>
+    <row r="57" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="37"/>
+      <c r="B57" s="21" t="s">
+        <v>293</v>
+      </c>
+      <c r="C57" s="37"/>
+      <c r="D57" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="F57" s="37"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="37"/>
+      <c r="J57" s="37"/>
+      <c r="K57" s="37"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="37"/>
+      <c r="B58" s="37"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="37"/>
+      <c r="I58" s="37"/>
+      <c r="J58" s="37"/>
+      <c r="K58" s="37"/>
+    </row>
+    <row r="59" customFormat="false" ht="127.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="37"/>
+      <c r="B59" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="C59" s="37"/>
+      <c r="D59" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>297</v>
+      </c>
+      <c r="G59" s="37"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="37"/>
+      <c r="J59" s="37"/>
+      <c r="K59" s="37"/>
+    </row>
+    <row r="60" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C60" s="0"/>
+      <c r="D60" s="21" t="s">
+        <v>298</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="F60" s="26" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="0"/>
+      <c r="D61" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="E61" s="21" t="s">
+        <v>302</v>
+      </c>
+      <c r="F61" s="26" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C62" s="0"/>
+      <c r="D62" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="E62" s="21" t="s">
+        <v>305</v>
+      </c>
+      <c r="F62" s="26" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="0"/>
+      <c r="C63" s="0"/>
+      <c r="D63" s="21" t="s">
+        <v>307</v>
+      </c>
+      <c r="E63" s="21" t="s">
+        <v>308</v>
+      </c>
+      <c r="F63" s="26" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="0"/>
+      <c r="C64" s="0"/>
+      <c r="D64" s="0"/>
+      <c r="E64" s="0"/>
+      <c r="F64" s="0"/>
+    </row>
+    <row r="65" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65" s="0"/>
+      <c r="D65" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="E65" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="F65" s="26" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C66" s="0"/>
+      <c r="D66" s="21" t="s">
+        <v>312</v>
+      </c>
+      <c r="E66" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="F66" s="26" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C67" s="0"/>
+      <c r="D67" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="E67" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F67" s="0"/>
+    </row>
+    <row r="68" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="C68" s="0"/>
+      <c r="D68" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="E68" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F68" s="0"/>
+    </row>
+    <row r="69" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="C69" s="0"/>
+      <c r="D69" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="E69" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F69" s="0"/>
+    </row>
+    <row r="70" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="C70" s="0"/>
+      <c r="D70" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="E70" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F70" s="0"/>
+    </row>
+    <row r="71" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="C71" s="0"/>
+      <c r="D71" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="E71" s="21" t="s">
+        <v>302</v>
+      </c>
+      <c r="F71" s="26" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="C72" s="0"/>
+      <c r="D72" s="21" t="s">
+        <v>316</v>
+      </c>
+      <c r="E72" s="21" t="s">
+        <v>302</v>
+      </c>
+      <c r="F72" s="26" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="0"/>
+      <c r="C73" s="0"/>
+      <c r="D73" s="0"/>
+      <c r="E73" s="0"/>
+      <c r="F73" s="0"/>
+    </row>
+    <row r="74" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="C74" s="21"/>
+      <c r="D74" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="E74" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="F74" s="26" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="21"/>
+      <c r="C75" s="21"/>
+      <c r="F75" s="0"/>
+    </row>
+    <row r="76" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="0"/>
+      <c r="C76" s="0"/>
+      <c r="D76" s="21" t="s">
+        <v>319</v>
+      </c>
+      <c r="E76" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="F76" s="0"/>
+    </row>
+    <row r="77" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="C77" s="21"/>
+      <c r="D77" s="21" t="s">
+        <v>321</v>
+      </c>
+      <c r="E77" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="F77" s="26" t="s">
+        <v>322</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="1:73"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3265,19 +4553,19 @@
       <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="38" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="20" t="s">
@@ -3297,19 +4585,19 @@
       <c r="B2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="26"/>
+      <c r="F2" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="38"/>
       <c r="H2" s="20" t="s">
         <v>16</v>
       </c>
@@ -3328,10 +4616,10 @@
       <c r="B3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="40" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="20" t="s">
@@ -3357,7 +4645,7 @@
       <c r="C4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="40" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="20" t="s">
@@ -3387,10 +4675,10 @@
       <c r="B5" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="40" t="s">
         <v>29</v>
       </c>
       <c r="E5" s="20" t="s">
@@ -3410,10 +4698,10 @@
       <c r="B6" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="40" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="20" t="s">
@@ -3433,10 +4721,10 @@
       <c r="B7" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="40" t="s">
         <v>36</v>
       </c>
       <c r="E7" s="20" t="s">
@@ -3459,10 +4747,10 @@
       <c r="B8" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="40" t="s">
         <v>42</v>
       </c>
       <c r="E8" s="20" t="s">
@@ -3483,10 +4771,10 @@
       <c r="B9" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="40" t="s">
         <v>46</v>
       </c>
       <c r="E9" s="20" t="s">
@@ -3512,7 +4800,7 @@
       <c r="C10" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="40" t="s">
         <v>55</v>
       </c>
       <c r="E10" s="20" t="s">
@@ -3570,7 +4858,7 @@
       <c r="C12" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="40" t="s">
         <v>64</v>
       </c>
       <c r="E12" s="20" t="s">
@@ -3596,7 +4884,7 @@
       <c r="C13" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="40" t="s">
         <v>67</v>
       </c>
       <c r="E13" s="20" t="s">
@@ -3626,7 +4914,7 @@
       <c r="C14" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="40" t="s">
         <v>71</v>
       </c>
       <c r="E14" s="20" t="s">
@@ -3649,7 +4937,7 @@
       <c r="C15" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="40" t="s">
         <v>73</v>
       </c>
       <c r="E15" s="20" t="s">
@@ -3674,7 +4962,7 @@
       <c r="C16" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="40" t="s">
         <v>76</v>
       </c>
       <c r="E16" s="20" t="s">
@@ -3700,7 +4988,7 @@
       <c r="C17" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="40" t="s">
         <v>79</v>
       </c>
       <c r="E17" s="20" t="s">
@@ -3730,7 +5018,7 @@
       <c r="C18" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="40" t="s">
         <v>83</v>
       </c>
       <c r="E18" s="20" t="s">
@@ -3757,7 +5045,7 @@
       <c r="C19" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="40" t="s">
         <v>87</v>
       </c>
       <c r="E19" s="20" t="s">
@@ -3786,7 +5074,7 @@
       <c r="C20" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="40" t="s">
         <v>91</v>
       </c>
       <c r="E20" s="20" t="s">
@@ -3835,7 +5123,7 @@
       <c r="C22" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="40" t="s">
         <v>108</v>
       </c>
       <c r="E22" s="25" t="s">
@@ -3864,7 +5152,7 @@
       <c r="C23" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="40" t="s">
         <v>115</v>
       </c>
       <c r="E23" s="20" t="s">
@@ -3888,7 +5176,7 @@
       <c r="C24" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="41" t="s">
         <v>117</v>
       </c>
       <c r="E24" s="20" t="s">
@@ -3906,7 +5194,7 @@
       <c r="C25" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="41" t="s">
         <v>120</v>
       </c>
       <c r="E25" s="20" t="s">
@@ -3924,7 +5212,7 @@
       <c r="C26" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="D26" s="29" t="s">
+      <c r="D26" s="41" t="s">
         <v>123</v>
       </c>
       <c r="E26" s="20" t="s">
@@ -3942,7 +5230,7 @@
       <c r="C27" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="40" t="s">
         <v>126</v>
       </c>
       <c r="E27" s="20" t="s">
@@ -3964,7 +5252,7 @@
       <c r="A28" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="D28" s="28"/>
+      <c r="D28" s="40"/>
       <c r="AMJ28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3975,7 +5263,7 @@
       <c r="C29" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="40" t="s">
         <v>130</v>
       </c>
       <c r="E29" s="20" t="s">
@@ -3996,7 +5284,7 @@
       <c r="C30" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="D30" s="28" t="s">
+      <c r="D30" s="40" t="s">
         <v>132</v>
       </c>
       <c r="E30" s="20" t="s">
@@ -4016,7 +5304,7 @@
       <c r="C31" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="D31" s="28" t="s">
+      <c r="D31" s="40" t="s">
         <v>134</v>
       </c>
       <c r="E31" s="20" t="s">
@@ -4038,7 +5326,7 @@
       <c r="C32" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="D32" s="28" t="s">
+      <c r="D32" s="40" t="s">
         <v>137</v>
       </c>
       <c r="E32" s="20" t="s">
@@ -4061,7 +5349,7 @@
       <c r="C33" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="D33" s="28" t="s">
+      <c r="D33" s="40" t="s">
         <v>140</v>
       </c>
       <c r="E33" s="20" t="s">
@@ -4087,7 +5375,7 @@
       <c r="C34" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="D34" s="28" t="s">
+      <c r="D34" s="40" t="s">
         <v>144</v>
       </c>
       <c r="E34" s="20" t="s">
@@ -4110,7 +5398,7 @@
       <c r="C35" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="D35" s="29" t="s">
+      <c r="D35" s="41" t="s">
         <v>147</v>
       </c>
       <c r="E35" s="20" t="s">
@@ -4127,7 +5415,7 @@
       <c r="C36" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D36" s="41" t="s">
         <v>149</v>
       </c>
       <c r="E36" s="20" t="s">
@@ -4147,7 +5435,7 @@
       <c r="C37" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="40" t="s">
         <v>152</v>
       </c>
       <c r="E37" s="20" t="s">
@@ -4166,7 +5454,7 @@
       <c r="C38" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="40" t="s">
         <v>154</v>
       </c>
       <c r="E38" s="20" t="s">
@@ -4185,7 +5473,7 @@
       <c r="C39" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="D39" s="28" t="s">
+      <c r="D39" s="40" t="s">
         <v>156</v>
       </c>
       <c r="E39" s="25" t="s">
@@ -4204,7 +5492,7 @@
       <c r="C40" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="D40" s="28" t="s">
+      <c r="D40" s="40" t="s">
         <v>159</v>
       </c>
       <c r="E40" s="25" t="s">
@@ -4223,7 +5511,7 @@
       <c r="C41" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="D41" s="28" t="s">
+      <c r="D41" s="40" t="s">
         <v>161</v>
       </c>
       <c r="E41" s="25" t="s">
@@ -4242,7 +5530,7 @@
       <c r="C42" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="D42" s="28" t="s">
+      <c r="D42" s="40" t="s">
         <v>163</v>
       </c>
       <c r="E42" s="25" t="s">
@@ -4261,7 +5549,7 @@
       <c r="C43" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="D43" s="28" t="s">
+      <c r="D43" s="40" t="s">
         <v>165</v>
       </c>
       <c r="E43" s="25" t="s">
@@ -4280,7 +5568,7 @@
       <c r="C44" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="D44" s="28" t="s">
+      <c r="D44" s="40" t="s">
         <v>167</v>
       </c>
       <c r="E44" s="25" t="s">
@@ -4299,7 +5587,7 @@
       <c r="C45" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="D45" s="28" t="s">
+      <c r="D45" s="40" t="s">
         <v>169</v>
       </c>
       <c r="E45" s="25" t="s">
@@ -4318,7 +5606,7 @@
       <c r="C46" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="D46" s="28" t="s">
+      <c r="D46" s="40" t="s">
         <v>171</v>
       </c>
       <c r="E46" s="25" t="s">
@@ -4337,7 +5625,7 @@
       <c r="C47" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="D47" s="28" t="s">
+      <c r="D47" s="40" t="s">
         <v>173</v>
       </c>
       <c r="E47" s="25" t="s">
@@ -4356,7 +5644,7 @@
       <c r="C48" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="D48" s="28" t="s">
+      <c r="D48" s="40" t="s">
         <v>175</v>
       </c>
       <c r="E48" s="25" t="s">
@@ -4375,7 +5663,7 @@
       <c r="C49" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="D49" s="28" t="s">
+      <c r="D49" s="40" t="s">
         <v>177</v>
       </c>
       <c r="E49" s="25" t="s">
@@ -4394,7 +5682,7 @@
       <c r="C50" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="D50" s="28" t="s">
+      <c r="D50" s="40" t="s">
         <v>179</v>
       </c>
       <c r="E50" s="25" t="s">
@@ -4413,7 +5701,7 @@
       <c r="C51" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="D51" s="28" t="s">
+      <c r="D51" s="40" t="s">
         <v>182</v>
       </c>
       <c r="E51" s="25" t="s">
@@ -4432,7 +5720,7 @@
       <c r="C52" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="D52" s="28" t="s">
+      <c r="D52" s="40" t="s">
         <v>184</v>
       </c>
       <c r="E52" s="25" t="s">
@@ -4451,7 +5739,7 @@
       <c r="C53" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="D53" s="28" t="s">
+      <c r="D53" s="40" t="s">
         <v>186</v>
       </c>
       <c r="E53" s="25" t="s">
@@ -4470,7 +5758,7 @@
       <c r="C54" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="D54" s="28" t="s">
+      <c r="D54" s="40" t="s">
         <v>188</v>
       </c>
       <c r="E54" s="25" t="s">
@@ -4489,7 +5777,7 @@
       <c r="C55" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="D55" s="28" t="s">
+      <c r="D55" s="40" t="s">
         <v>190</v>
       </c>
       <c r="E55" s="25" t="s">
@@ -4508,7 +5796,7 @@
       <c r="C56" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="D56" s="28" t="s">
+      <c r="D56" s="40" t="s">
         <v>192</v>
       </c>
       <c r="E56" s="25" t="s">
@@ -4527,7 +5815,7 @@
       <c r="C57" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D57" s="28" t="s">
+      <c r="D57" s="40" t="s">
         <v>194</v>
       </c>
       <c r="E57" s="25" t="s">
@@ -4546,7 +5834,7 @@
       <c r="C58" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="D58" s="28" t="s">
+      <c r="D58" s="40" t="s">
         <v>196</v>
       </c>
       <c r="E58" s="25" t="s">
@@ -4565,7 +5853,7 @@
       <c r="C59" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="D59" s="28" t="s">
+      <c r="D59" s="40" t="s">
         <v>198</v>
       </c>
       <c r="E59" s="25" t="s">
@@ -4584,7 +5872,7 @@
       <c r="C60" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="D60" s="28" t="s">
+      <c r="D60" s="40" t="s">
         <v>200</v>
       </c>
       <c r="E60" s="25" t="s">
@@ -4603,7 +5891,7 @@
       <c r="C61" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="D61" s="28" t="s">
+      <c r="D61" s="40" t="s">
         <v>202</v>
       </c>
       <c r="E61" s="25" t="s">
@@ -4622,7 +5910,7 @@
       <c r="C62" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="D62" s="28" t="s">
+      <c r="D62" s="40" t="s">
         <v>204</v>
       </c>
       <c r="E62" s="25" t="s">
@@ -4641,7 +5929,7 @@
       <c r="C63" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="D63" s="28" t="s">
+      <c r="D63" s="40" t="s">
         <v>206</v>
       </c>
       <c r="E63" s="25" t="s">
@@ -4660,7 +5948,7 @@
       <c r="C64" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="D64" s="28" t="s">
+      <c r="D64" s="40" t="s">
         <v>208</v>
       </c>
       <c r="E64" s="25" t="s">
@@ -4679,7 +5967,7 @@
       <c r="C65" s="20" t="s">
         <v>209</v>
       </c>
-      <c r="D65" s="28" t="s">
+      <c r="D65" s="40" t="s">
         <v>210</v>
       </c>
       <c r="E65" s="20" t="s">
@@ -4698,7 +5986,7 @@
       <c r="C66" s="20" t="s">
         <v>212</v>
       </c>
-      <c r="D66" s="28" t="s">
+      <c r="D66" s="40" t="s">
         <v>213</v>
       </c>
       <c r="E66" s="20" t="s">
@@ -4717,7 +6005,7 @@
       <c r="C67" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="D67" s="28" t="s">
+      <c r="D67" s="40" t="s">
         <v>215</v>
       </c>
       <c r="E67" s="20" t="s">
@@ -4736,7 +6024,7 @@
       <c r="C68" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="D68" s="28" t="s">
+      <c r="D68" s="40" t="s">
         <v>217</v>
       </c>
       <c r="E68" s="20" t="s">
@@ -4755,7 +6043,7 @@
       <c r="C69" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D69" s="28" t="s">
+      <c r="D69" s="40" t="s">
         <v>219</v>
       </c>
       <c r="E69" s="20" t="s">
@@ -4782,7 +6070,7 @@
       <c r="C70" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="D70" s="28" t="s">
+      <c r="D70" s="40" t="s">
         <v>223</v>
       </c>
       <c r="E70" s="20" t="s">
@@ -4807,7 +6095,7 @@
       <c r="C71" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="D71" s="28" t="s">
+      <c r="D71" s="40" t="s">
         <v>227</v>
       </c>
       <c r="E71" s="20" t="s">
@@ -4831,7 +6119,7 @@
       <c r="C72" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="D72" s="28" t="s">
+      <c r="D72" s="40" t="s">
         <v>228</v>
       </c>
       <c r="E72" s="20" t="s">
@@ -4855,7 +6143,7 @@
       <c r="C73" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="D73" s="28" t="s">
+      <c r="D73" s="40" t="s">
         <v>230</v>
       </c>
       <c r="E73" s="20" t="s">

</xml_diff>